<commit_message>
reformulation and ccg for robust facility location
</commit_message>
<xml_diff>
--- a/Multiknapsack/M1_N5_T6_a25_ccg.xlsx
+++ b/Multiknapsack/M1_N5_T6_a25_ccg.xlsx
@@ -465,7 +465,7 @@
         <v>-5.143583366953895</v>
       </c>
       <c r="C2">
-        <v>0.33103301144409175</v>
+        <v>0.28012913242492676</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -491,7 +491,7 @@
         <v>-4.794537358217317</v>
       </c>
       <c r="C3">
-        <v>0.01204913542175293</v>
+        <v>0.018531504904174805</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -517,7 +517,7 @@
         <v>-4.5385873718839385</v>
       </c>
       <c r="C4">
-        <v>0.04976727629394531</v>
+        <v>0.051866531335449224</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -543,7 +543,7 @@
         <v>-7.269329605163567</v>
       </c>
       <c r="C5">
-        <v>0.04128934087219238</v>
+        <v>0.037267592370605465</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -569,7 +569,7 @@
         <v>-7.801849740518528</v>
       </c>
       <c r="C6">
-        <v>0.01567671798400879</v>
+        <v>0.016084083923339845</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -595,7 +595,7 @@
         <v>-9.729886293229871</v>
       </c>
       <c r="C7">
-        <v>0.013427962942504883</v>
+        <v>0.004594</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -621,7 +621,7 @@
         <v>-5.069880159121121</v>
       </c>
       <c r="C8">
-        <v>0.01832393896484375</v>
+        <v>0.022605987466430662</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -647,7 +647,7 @@
         <v>-6.930429815339221</v>
       </c>
       <c r="C9">
-        <v>0.012004097003173828</v>
+        <v>0.022793714987182617</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -673,7 +673,7 @@
         <v>-2.847381425048557</v>
       </c>
       <c r="C10">
-        <v>0.022371487466430664</v>
+        <v>0.02160045994567871</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -699,7 +699,7 @@
         <v>-10.1902783475591</v>
       </c>
       <c r="C11">
-        <v>0.028297829428100586</v>
+        <v>0.027809729428100588</v>
       </c>
       <c r="D11">
         <v>2</v>

</xml_diff>